<commit_message>
Investigation write-ups and more file assets
</commit_message>
<xml_diff>
--- a/a_place_for_salvador_allende_raw.xlsx
+++ b/a_place_for_salvador_allende_raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\datasets-of-interest\a-place-for-salvador-allende\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\a-place-for-salvador-allende\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D880C955-1F46-4B2A-ABB5-7D00F86C7F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05755C0-E65C-4A18-BA8F-3EF257B534E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14178,10 +14178,10 @@
   <dimension ref="A1:AO781"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M68" sqref="M68"/>
+      <selection pane="bottomRight" activeCell="K185" sqref="K185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -25763,10 +25763,10 @@
         <v>2005</v>
       </c>
       <c r="L185" s="2">
-        <v>10.276966835161099</v>
+        <v>10.2769935299275</v>
       </c>
       <c r="M185" s="2">
-        <v>10.276966835161099</v>
+        <v>-68.006670223313094</v>
       </c>
       <c r="N185" s="2">
         <v>2007</v>

</xml_diff>

<commit_message>
Username update and additional data
</commit_message>
<xml_diff>
--- a/a_place_for_salvador_allende_raw.xlsx
+++ b/a_place_for_salvador_allende_raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\a-place-for-salvador-allende\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170E4772-80C7-4810-8A13-952E4832DC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E711BDE9-DA70-443D-85EF-6F34B6A4FCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10521" uniqueCount="4414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10532" uniqueCount="4421">
   <si>
     <t>id</t>
   </si>
@@ -13907,6 +13907,27 @@
   </si>
   <si>
     <t>Türkiye</t>
+  </si>
+  <si>
+    <t>S. Allendeplein</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/6398894</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/rucZv3wDT9XHMDxh9</t>
+  </si>
+  <si>
+    <t>Groningen</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Hoornse Meer</t>
+  </si>
+  <si>
+    <t>9728 TK</t>
   </si>
 </sst>
 </file>
@@ -14237,10 +14258,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AO784"/>
+  <dimension ref="A1:AO785"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B760" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B774" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A785" sqref="A785"/>
@@ -64064,11 +64085,67 @@
       <c r="V784" s="2">
         <v>1</v>
       </c>
-      <c r="W784" s="11" t="s">
+      <c r="W784" s="2" t="s">
         <v>4410</v>
       </c>
-      <c r="X784" s="11" t="s">
+      <c r="X784" s="2" t="s">
         <v>4409</v>
+      </c>
+    </row>
+    <row r="785" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A785" s="2">
+        <v>784</v>
+      </c>
+      <c r="B785" s="2" t="s">
+        <v>4414</v>
+      </c>
+      <c r="C785" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D785" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E785" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="F785" s="2" t="s">
+        <v>4417</v>
+      </c>
+      <c r="G785" s="2" t="s">
+        <v>4418</v>
+      </c>
+      <c r="H785" s="2" t="s">
+        <v>4419</v>
+      </c>
+      <c r="K785" s="8" t="s">
+        <v>4420</v>
+      </c>
+      <c r="L785" s="2">
+        <v>53.187083000000001</v>
+      </c>
+      <c r="M785" s="2">
+        <v>6.5580499999999997</v>
+      </c>
+      <c r="N785" s="2">
+        <v>2007</v>
+      </c>
+      <c r="O785" s="2">
+        <v>9</v>
+      </c>
+      <c r="P785" s="2">
+        <v>17</v>
+      </c>
+      <c r="Q785" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="V785" s="2">
+        <v>1</v>
+      </c>
+      <c r="W785" s="2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="X785" s="2" t="s">
+        <v>4416</v>
       </c>
     </row>
   </sheetData>
@@ -64318,10 +64395,12 @@
     <hyperlink ref="X782" r:id="rId239" xr:uid="{EF6C3DD7-4009-4EDA-970B-927C0BF0F346}"/>
     <hyperlink ref="X783" r:id="rId240" xr:uid="{2489D1B4-78B7-429C-A638-2602E7231287}"/>
     <hyperlink ref="W783" r:id="rId241" xr:uid="{F54A0F1F-897B-4DF9-87B1-239130029A7E}"/>
-    <hyperlink ref="W784" r:id="rId242" xr:uid="{A04E8472-B4B9-4BA1-9A47-D3D214B158AC}"/>
-    <hyperlink ref="X784" r:id="rId243" xr:uid="{82864AB8-9C9E-4145-A962-85712CA17543}"/>
+    <hyperlink ref="X785" r:id="rId242" xr:uid="{6CC16959-B03E-4BAA-A717-6C2A3051CA92}"/>
+    <hyperlink ref="W785" r:id="rId243" xr:uid="{C8C65B0B-24E5-4936-9D68-A68D793F0AA6}"/>
+    <hyperlink ref="X784" r:id="rId244" xr:uid="{82864AB8-9C9E-4145-A962-85712CA17543}"/>
+    <hyperlink ref="W784" r:id="rId245" xr:uid="{A04E8472-B4B9-4BA1-9A47-D3D214B158AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId244"/>
+  <pageSetup orientation="portrait" r:id="rId246"/>
 </worksheet>
 </file>
</xml_diff>